<commit_message>
Updates as of 7/6/2022
</commit_message>
<xml_diff>
--- a/SPT Config Generator.xlsx
+++ b/SPT Config Generator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wblankenship\Documents\GitHub\SPT-Builder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE26B7E0-4EF8-4E5E-B58B-80DF0F4673F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3965754-1753-4627-AC79-42B2419DFE2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D2F1E244-0055-49E9-BA99-E37AFD162BFC}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="39">
   <si>
     <t>SPARE</t>
   </si>
@@ -75,52 +75,79 @@
     <t>Momentary Change Detect (MCD) OR  2 Bit Binary (2B) OR (II)</t>
   </si>
   <si>
-    <t>BK 1&amp;2 OIL SPL</t>
-  </si>
-  <si>
-    <t>Z104-1 LBSW</t>
-  </si>
-  <si>
-    <t>Z104-2 LBSW</t>
-  </si>
-  <si>
-    <t>TRIPPING DC</t>
-  </si>
-  <si>
-    <t>43175 OCB</t>
-  </si>
-  <si>
-    <t>43176 OCB</t>
-  </si>
-  <si>
-    <t>43484 OCB</t>
-  </si>
-  <si>
-    <t>UNDEFINED</t>
-  </si>
-  <si>
     <t>CLOSE</t>
   </si>
   <si>
     <t>OPEN</t>
   </si>
   <si>
-    <t xml:space="preserve"> 43484 MW</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 43484 MVAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 43175 MW</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 43175 MVAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This Point is cool </t>
-  </si>
-  <si>
-    <t xml:space="preserve">This point is cool </t>
+    <t>ADAPTIVE RELAYING</t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>BANK 1 MW</t>
+  </si>
+  <si>
+    <t>BANK 1 MVAR</t>
+  </si>
+  <si>
+    <t>BANK 2 MW</t>
+  </si>
+  <si>
+    <t>BANK 2 MVAR</t>
+  </si>
+  <si>
+    <t>Frame/Sequence</t>
+  </si>
+  <si>
+    <t>M139-1 LBSW</t>
+  </si>
+  <si>
+    <t>NO 6 LBSW</t>
+  </si>
+  <si>
+    <t>M139-2 LBSW</t>
+  </si>
+  <si>
+    <t>BK 1</t>
+  </si>
+  <si>
+    <t>BK 2</t>
+  </si>
+  <si>
+    <t>5PCT VOLT RED</t>
+  </si>
+  <si>
+    <t>BK 1 VCB</t>
+  </si>
+  <si>
+    <t>BT VCB</t>
+  </si>
+  <si>
+    <t>47426 VCB</t>
+  </si>
+  <si>
+    <t>47427 VCB</t>
+  </si>
+  <si>
+    <t>BK 2 VCB</t>
+  </si>
+  <si>
+    <t>47428 VCB</t>
+  </si>
+  <si>
+    <t>47429 VCB</t>
+  </si>
+  <si>
+    <t>Undefined</t>
+  </si>
+  <si>
+    <t>BANK 2 kV</t>
   </si>
 </sst>
 </file>
@@ -513,22 +540,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A9C7EB-CAA4-4DB0-AECE-FAF550B5EE12}">
   <dimension ref="B2:R186"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42.28515625" customWidth="1"/>
     <col min="5" max="5" width="2.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="34.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2.7109375" customWidth="1"/>
     <col min="10" max="10" width="14.42578125" customWidth="1"/>
     <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="2.7109375" customWidth="1"/>
     <col min="15" max="15" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -563,7 +590,7 @@
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
@@ -572,7 +599,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>7</v>
@@ -605,17 +632,17 @@
       <c r="R3" s="3"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4" s="8">
-        <v>32</v>
+      <c r="B4" s="6">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6">
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F4" s="6">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G4" s="8">
         <v>0</v>
@@ -624,19 +651,19 @@
         <v>11</v>
       </c>
       <c r="J4" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" s="4">
         <v>0</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="M4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="O4" s="4">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="P4" s="4">
         <v>0</v>
@@ -647,17 +674,17 @@
       <c r="R4" s="2"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5" s="8">
-        <v>33</v>
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6">
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F5" s="6">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G5" s="8">
         <v>1</v>
@@ -666,19 +693,19 @@
         <v>10</v>
       </c>
       <c r="J5" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5" s="4">
         <v>0</v>
       </c>
       <c r="L5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" t="s">
         <v>15</v>
       </c>
-      <c r="M5" t="s">
-        <v>23</v>
-      </c>
       <c r="O5" s="4">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="P5" s="4">
         <v>1</v>
@@ -689,424 +716,374 @@
       <c r="R5" s="2"/>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6" s="8">
-        <v>34</v>
+      <c r="B6" s="6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="6">
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="F6" s="6">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G6" s="8">
         <v>2</v>
       </c>
       <c r="H6" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="J6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6" s="4">
         <v>1</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="M6" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="O6" s="4">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="P6" s="4">
         <v>2</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="R6" s="2"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7" s="8">
-        <v>35</v>
+      <c r="B7" s="6">
+        <v>0</v>
+      </c>
+      <c r="C7" s="6">
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="F7" s="6">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G7" s="8">
         <v>3</v>
       </c>
       <c r="H7" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="J7" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7" s="4">
         <v>1</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="M7" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="O7" s="4">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="P7" s="4">
         <v>3</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="R7" s="2"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8" s="8">
-        <v>36</v>
+      <c r="B8" s="6">
+        <v>0</v>
+      </c>
+      <c r="C8" s="6">
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="F8" s="6">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G8" s="8">
         <v>4</v>
       </c>
       <c r="H8" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="J8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8" s="4">
         <v>2</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="M8" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="O8" s="4">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="P8" s="4">
         <v>4</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="R8" s="2"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9" s="8">
-        <v>37</v>
+      <c r="B9" s="6">
+        <v>0</v>
+      </c>
+      <c r="C9" s="6">
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="F9" s="6">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G9" s="8">
         <v>5</v>
       </c>
       <c r="H9" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="J9" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9" s="4">
         <v>2</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="M9" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="O9" s="4">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="P9" s="4">
         <v>5</v>
       </c>
       <c r="Q9" s="7" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="R9" s="2"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10" s="8">
-        <v>38</v>
+      <c r="B10" s="6">
+        <v>0</v>
+      </c>
+      <c r="C10" s="6">
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="F10" s="6">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G10" s="8">
         <v>6</v>
       </c>
       <c r="H10" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="J10" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10" s="4">
         <v>3</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="M10" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="O10" s="4">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="P10" s="4">
         <v>6</v>
       </c>
       <c r="Q10" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="R10" s="2"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11" s="8">
-        <v>39</v>
+      <c r="B11" s="6">
+        <v>0</v>
+      </c>
+      <c r="C11" s="6">
+        <v>23</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
       </c>
       <c r="F11" s="6">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G11" s="8">
         <v>7</v>
       </c>
       <c r="H11" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="J11" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11" s="4">
         <v>3</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="M11" t="s">
-        <v>23</v>
-      </c>
-      <c r="O11" s="4">
-        <v>0</v>
-      </c>
-      <c r="P11" s="4">
-        <v>7</v>
-      </c>
-      <c r="Q11" s="7" t="s">
-        <v>21</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="7"/>
       <c r="R11" s="2"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" s="8">
-        <v>40</v>
+      <c r="B12" s="6">
+        <v>0</v>
+      </c>
+      <c r="C12" s="6">
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="F12" s="6">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G12" s="8">
         <v>8</v>
       </c>
       <c r="H12" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="J12" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K12" s="4">
         <v>4</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="M12" t="s">
-        <v>22</v>
-      </c>
-      <c r="O12" s="4">
-        <v>0</v>
-      </c>
-      <c r="P12" s="4">
-        <v>8</v>
-      </c>
-      <c r="Q12" s="7" t="s">
-        <v>24</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="7"/>
       <c r="R12" s="2"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" s="8">
-        <v>41</v>
-      </c>
-      <c r="D13" t="s">
-        <v>19</v>
-      </c>
+      <c r="B13" s="6"/>
       <c r="F13" s="6">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G13" s="8">
         <v>9</v>
       </c>
       <c r="H13" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="J13" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13" s="4">
         <v>4</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="M13" t="s">
-        <v>23</v>
-      </c>
-      <c r="O13" s="4">
-        <v>0</v>
-      </c>
-      <c r="P13" s="4">
-        <v>9</v>
-      </c>
-      <c r="Q13" s="7" t="s">
-        <v>25</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="7"/>
       <c r="R13" s="2"/>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" s="8">
-        <v>42</v>
-      </c>
-      <c r="D14" t="s">
-        <v>20</v>
-      </c>
+      <c r="B14" s="6"/>
       <c r="F14" s="6">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G14" s="8">
         <v>10</v>
       </c>
       <c r="H14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J14" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14" s="4">
         <v>5</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="O14" s="4">
-        <v>0</v>
-      </c>
-      <c r="P14" s="4">
-        <v>10</v>
-      </c>
-      <c r="Q14" s="7" t="s">
-        <v>26</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="M14" t="s">
+        <v>14</v>
+      </c>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="7"/>
       <c r="R14" s="2"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" s="8">
-        <v>43</v>
-      </c>
-      <c r="D15" t="s">
-        <v>0</v>
-      </c>
+      <c r="B15" s="6"/>
       <c r="F15" s="6">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G15" s="8">
         <v>11</v>
       </c>
       <c r="H15" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="J15" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15" s="4">
         <v>5</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>21</v>
+        <v>32</v>
+      </c>
+      <c r="M15" t="s">
+        <v>15</v>
       </c>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="R15" s="2"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" s="8">
-        <v>44</v>
-      </c>
-      <c r="D16" t="s">
-        <v>0</v>
-      </c>
+      <c r="B16" s="6"/>
       <c r="F16" s="6">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G16" s="8">
         <v>12</v>
@@ -1115,29 +1092,24 @@
         <v>0</v>
       </c>
       <c r="J16" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16" s="4">
         <v>6</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>21</v>
+        <v>33</v>
+      </c>
+      <c r="M16" t="s">
+        <v>14</v>
       </c>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" s="8">
-        <v>45</v>
-      </c>
-      <c r="D17" t="s">
-        <v>0</v>
-      </c>
+      <c r="B17" s="6"/>
       <c r="F17" s="6">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G17" s="8">
         <v>13</v>
@@ -1146,29 +1118,24 @@
         <v>0</v>
       </c>
       <c r="J17" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17" s="4">
         <v>6</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>21</v>
+        <v>33</v>
+      </c>
+      <c r="M17" t="s">
+        <v>15</v>
       </c>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" s="8">
-        <v>46</v>
-      </c>
-      <c r="D18" t="s">
-        <v>0</v>
-      </c>
+      <c r="B18" s="6"/>
       <c r="F18" s="6">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G18" s="8">
         <v>14</v>
@@ -1177,29 +1144,24 @@
         <v>0</v>
       </c>
       <c r="J18" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K18" s="4">
         <v>7</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>21</v>
+        <v>34</v>
+      </c>
+      <c r="M18" t="s">
+        <v>14</v>
       </c>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" s="8">
-        <v>47</v>
-      </c>
-      <c r="D19" t="s">
-        <v>0</v>
-      </c>
+      <c r="B19" s="6"/>
       <c r="F19" s="6">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G19" s="8">
         <v>15</v>
@@ -1209,400 +1171,305 @@
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19" s="4">
         <v>7</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>21</v>
+        <v>34</v>
+      </c>
+      <c r="M19" t="s">
+        <v>15</v>
       </c>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B20" s="6">
-        <v>1</v>
-      </c>
-      <c r="C20" s="8">
-        <v>48</v>
-      </c>
-      <c r="D20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="6">
-        <v>1</v>
-      </c>
-      <c r="G20" s="8">
-        <v>16</v>
-      </c>
-      <c r="H20" t="s">
-        <v>28</v>
-      </c>
+      <c r="B20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="8"/>
       <c r="I20" s="2"/>
       <c r="J20" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K20" s="4">
         <v>8</v>
       </c>
       <c r="L20" s="7" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M20" t="s">
-        <v>22</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="O20" s="4"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="F21" s="6">
-        <v>1</v>
-      </c>
-      <c r="G21" s="8">
-        <v>17</v>
-      </c>
-      <c r="H21" t="s">
-        <v>10</v>
-      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="8"/>
       <c r="I21" s="2"/>
       <c r="J21" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K21" s="4">
         <v>8</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M21" t="s">
-        <v>23</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="O21" s="4"/>
       <c r="Q21" s="1"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="F22" s="6">
-        <v>1</v>
-      </c>
-      <c r="G22" s="8">
-        <v>18</v>
-      </c>
-      <c r="H22" t="s">
-        <v>14</v>
-      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="8"/>
       <c r="I22" s="2"/>
       <c r="J22" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K22" s="4">
         <v>9</v>
       </c>
       <c r="L22" s="7" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="M22" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="Q22" s="1"/>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="F23" s="6">
-        <v>1</v>
-      </c>
-      <c r="G23" s="8">
-        <v>19</v>
-      </c>
-      <c r="H23" t="s">
-        <v>15</v>
-      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="8"/>
       <c r="I23" s="2"/>
       <c r="J23" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K23" s="4">
         <v>9</v>
       </c>
       <c r="L23" s="7" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="M23" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="F24" s="6">
-        <v>1</v>
-      </c>
-      <c r="G24" s="8">
-        <v>20</v>
-      </c>
-      <c r="H24" t="s">
-        <v>15</v>
-      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="8"/>
       <c r="I24" s="2"/>
       <c r="J24" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K24" s="4">
         <v>10</v>
       </c>
       <c r="L24" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M24" t="s">
         <v>18</v>
-      </c>
-      <c r="M24" t="s">
-        <v>22</v>
       </c>
       <c r="O24" s="2"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="2"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="F25" s="6">
-        <v>1</v>
-      </c>
-      <c r="G25" s="8">
-        <v>21</v>
-      </c>
-      <c r="H25" t="s">
-        <v>16</v>
-      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="8"/>
       <c r="I25" s="2"/>
       <c r="J25" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K25" s="4">
         <v>10</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M25" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="O25" s="2"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="2"/>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="F26" s="6">
-        <v>1</v>
-      </c>
-      <c r="G26" s="8">
-        <v>22</v>
-      </c>
-      <c r="H26" t="s">
-        <v>16</v>
-      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="8"/>
       <c r="I26" s="2"/>
       <c r="J26" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K26" s="4">
         <v>11</v>
       </c>
       <c r="L26" s="7" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="M26" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="O26" s="2"/>
       <c r="P26" s="4"/>
       <c r="Q26" s="2"/>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="F27" s="6">
-        <v>1</v>
-      </c>
-      <c r="G27" s="8">
-        <v>23</v>
-      </c>
-      <c r="H27" t="s">
-        <v>17</v>
-      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="8"/>
       <c r="I27" s="2"/>
       <c r="J27" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K27" s="4">
         <v>11</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="M27" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="O27" s="2"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="2"/>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="F28" s="6">
-        <v>1</v>
-      </c>
-      <c r="G28" s="8">
-        <v>24</v>
-      </c>
-      <c r="H28" t="s">
-        <v>0</v>
-      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="8"/>
       <c r="I28" s="2"/>
       <c r="J28" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K28" s="4">
         <v>12</v>
       </c>
       <c r="L28" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="M28" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="F29" s="6">
-        <v>1</v>
-      </c>
-      <c r="G29" s="8">
-        <v>25</v>
-      </c>
-      <c r="H29" t="s">
-        <v>0</v>
-      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="8"/>
       <c r="J29" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K29" s="4">
         <v>12</v>
       </c>
       <c r="L29" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="M29" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="F30" s="6">
-        <v>1</v>
-      </c>
-      <c r="G30" s="8">
-        <v>26</v>
-      </c>
-      <c r="H30" t="s">
-        <v>0</v>
-      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="8"/>
       <c r="J30" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K30" s="4">
         <v>13</v>
       </c>
       <c r="L30" s="7" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="F31" s="6">
-        <v>1</v>
-      </c>
-      <c r="G31" s="8">
-        <v>27</v>
-      </c>
-      <c r="H31" t="s">
-        <v>0</v>
-      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="8"/>
       <c r="J31" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K31" s="4">
         <v>13</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="F32" s="6">
-        <v>1</v>
-      </c>
-      <c r="G32" s="8">
-        <v>28</v>
-      </c>
-      <c r="H32" t="s">
-        <v>0</v>
-      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="8"/>
       <c r="J32" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K32" s="4">
         <v>14</v>
       </c>
       <c r="L32" s="7" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="F33" s="6">
-        <v>1</v>
-      </c>
-      <c r="G33" s="8">
-        <v>29</v>
-      </c>
-      <c r="H33" t="s">
-        <v>0</v>
-      </c>
+      <c r="F33" s="6"/>
+      <c r="G33" s="8"/>
       <c r="J33" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K33" s="4">
         <v>14</v>
       </c>
       <c r="L33" s="7" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="F34" s="6">
-        <v>1</v>
-      </c>
-      <c r="G34" s="8">
-        <v>30</v>
-      </c>
-      <c r="H34" t="s">
-        <v>0</v>
-      </c>
+      <c r="F34" s="6"/>
+      <c r="G34" s="8"/>
       <c r="J34" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K34" s="4">
         <v>15</v>
       </c>
       <c r="L34" s="7" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="F35" s="6">
-        <v>1</v>
-      </c>
-      <c r="G35" s="8">
-        <v>31</v>
-      </c>
-      <c r="H35" t="s">
-        <v>0</v>
-      </c>
+      <c r="F35" s="6"/>
+      <c r="G35" s="8"/>
       <c r="J35" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K35" s="4">
         <v>15</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="F36" s="6"/>
+      <c r="G36" s="8"/>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
       <c r="L36" s="7"/>
@@ -1610,7 +1477,7 @@
     <row r="37" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
       <c r="C37" s="5"/>
-      <c r="F37" s="4"/>
+      <c r="F37" s="6"/>
       <c r="G37" s="4"/>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
@@ -1620,7 +1487,7 @@
     <row r="38" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
       <c r="C38" s="5"/>
-      <c r="F38" s="4"/>
+      <c r="F38" s="6"/>
       <c r="G38" s="4"/>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
@@ -1630,7 +1497,7 @@
     <row r="39" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
       <c r="C39" s="5"/>
-      <c r="F39" s="4"/>
+      <c r="F39" s="6"/>
       <c r="G39" s="4"/>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
@@ -1639,7 +1506,7 @@
     <row r="40" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
       <c r="C40" s="5"/>
-      <c r="F40" s="4"/>
+      <c r="F40" s="6"/>
       <c r="G40" s="4"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
@@ -1648,7 +1515,7 @@
     <row r="41" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
       <c r="C41" s="5"/>
-      <c r="F41" s="4"/>
+      <c r="F41" s="6"/>
       <c r="G41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
@@ -1657,7 +1524,7 @@
     <row r="42" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="5"/>
-      <c r="F42" s="4"/>
+      <c r="F42" s="6"/>
       <c r="G42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
@@ -1666,7 +1533,7 @@
     <row r="43" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="5"/>
-      <c r="F43" s="4"/>
+      <c r="F43" s="6"/>
       <c r="G43" s="4"/>
       <c r="H43" s="7"/>
       <c r="J43" s="4"/>
@@ -1676,7 +1543,7 @@
     <row r="44" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B44" s="2"/>
       <c r="C44" s="5"/>
-      <c r="F44" s="4"/>
+      <c r="F44" s="6"/>
       <c r="G44" s="4"/>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
@@ -1685,7 +1552,7 @@
     <row r="45" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B45" s="2"/>
       <c r="C45" s="5"/>
-      <c r="F45" s="4"/>
+      <c r="F45" s="6"/>
       <c r="G45" s="4"/>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
@@ -1694,7 +1561,7 @@
     <row r="46" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B46" s="2"/>
       <c r="C46" s="5"/>
-      <c r="F46" s="4"/>
+      <c r="F46" s="6"/>
       <c r="G46" s="4"/>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
@@ -1703,7 +1570,7 @@
     <row r="47" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
       <c r="C47" s="5"/>
-      <c r="F47" s="4"/>
+      <c r="F47" s="6"/>
       <c r="G47" s="4"/>
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
@@ -1712,7 +1579,7 @@
     <row r="48" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B48" s="2"/>
       <c r="C48" s="5"/>
-      <c r="F48" s="4"/>
+      <c r="F48" s="6"/>
       <c r="G48" s="4"/>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
@@ -1721,7 +1588,7 @@
     <row r="49" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
       <c r="C49" s="5"/>
-      <c r="F49" s="4"/>
+      <c r="F49" s="6"/>
       <c r="G49" s="4"/>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
@@ -1730,7 +1597,7 @@
     <row r="50" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
       <c r="C50" s="5"/>
-      <c r="F50" s="4"/>
+      <c r="F50" s="6"/>
       <c r="G50" s="4"/>
       <c r="H50" s="7"/>
       <c r="J50" s="4"/>
@@ -1740,7 +1607,7 @@
     <row r="51" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B51" s="2"/>
       <c r="C51" s="5"/>
-      <c r="F51" s="4"/>
+      <c r="F51" s="6"/>
       <c r="G51" s="4"/>
       <c r="H51" s="7"/>
       <c r="J51" s="4"/>
@@ -1750,56 +1617,56 @@
     <row r="52" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B52" s="2"/>
       <c r="C52" s="5"/>
-      <c r="F52" s="4"/>
+      <c r="F52" s="6"/>
       <c r="G52" s="4"/>
       <c r="H52" s="7"/>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B53" s="2"/>
       <c r="C53" s="5"/>
-      <c r="F53" s="4"/>
+      <c r="F53" s="6"/>
       <c r="G53" s="4"/>
       <c r="H53" s="7"/>
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B54" s="2"/>
       <c r="C54" s="5"/>
-      <c r="F54" s="4"/>
+      <c r="F54" s="6"/>
       <c r="G54" s="4"/>
       <c r="H54" s="7"/>
     </row>
     <row r="55" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B55" s="2"/>
       <c r="C55" s="5"/>
-      <c r="F55" s="4"/>
+      <c r="F55" s="6"/>
       <c r="G55" s="4"/>
       <c r="H55" s="7"/>
     </row>
     <row r="56" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B56" s="2"/>
       <c r="C56" s="5"/>
-      <c r="F56" s="4"/>
+      <c r="F56" s="6"/>
       <c r="G56" s="4"/>
       <c r="H56" s="7"/>
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B57" s="2"/>
       <c r="C57" s="5"/>
-      <c r="F57" s="4"/>
+      <c r="F57" s="6"/>
       <c r="G57" s="4"/>
       <c r="H57" s="7"/>
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B58" s="2"/>
       <c r="C58" s="5"/>
-      <c r="F58" s="4"/>
+      <c r="F58" s="6"/>
       <c r="G58" s="4"/>
       <c r="H58" s="7"/>
     </row>
     <row r="59" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B59" s="2"/>
       <c r="C59" s="5"/>
-      <c r="F59" s="4"/>
+      <c r="F59" s="6"/>
       <c r="G59" s="4"/>
       <c r="H59" s="7"/>
     </row>

</xml_diff>